<commit_message>
feat[pm]: checked registers and charter
</commit_message>
<xml_diff>
--- a/project-managment/lab-2/Реестр заинтересованных сторон.xlsx
+++ b/project-managment/lab-2/Реестр заинтересованных сторон.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RobotComp.ru\Desktop\labs-4-course\project-managment\lab-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711C1984-AF21-416F-A4BC-99EA01DAEEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA7405C-F3F6-4C32-89E8-1124A5CAA412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,12 +162,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -176,13 +173,13 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -220,17 +217,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AA0F6F66-5D02-4C1A-94D6-198FC666F3D2}" name="Таблица1" displayName="Таблица1" ref="A1:H8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AA0F6F66-5D02-4C1A-94D6-198FC666F3D2}" name="Таблица1" displayName="Таблица1" ref="A1:H8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H8" xr:uid="{AA0F6F66-5D02-4C1A-94D6-198FC666F3D2}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{19E8CA66-A18E-49C5-B681-EAE1041137E1}" name="№" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{CB0AB4A5-2670-4FC6-B1B6-9D9822F897E0}" name="ФИО/Организация" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6DE3E606-CF69-4A11-805E-D498690FDCAC}" name="Роль" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{651BC2FF-A11D-4CF7-BF24-2415EFE50C5C}" name="Влияние" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{9CBF190A-2384-473E-9476-07D272A20FED}" name="Влияние (пояснение)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{856B7D9E-43DD-4D4C-BC39-6C3935D8163A}" name="Интерес" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{A897308E-A602-47B1-B48B-4FD470549A10}" name="Интерес (пояснение)" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{C64844D7-2D5C-4311-9B26-83BA3A81B513}" name="Выбранная стратегия" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{19E8CA66-A18E-49C5-B681-EAE1041137E1}" name="№" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{CB0AB4A5-2670-4FC6-B1B6-9D9822F897E0}" name="ФИО/Организация" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{6DE3E606-CF69-4A11-805E-D498690FDCAC}" name="Роль" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{651BC2FF-A11D-4CF7-BF24-2415EFE50C5C}" name="Влияние" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{9CBF190A-2384-473E-9476-07D272A20FED}" name="Влияние (пояснение)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{856B7D9E-43DD-4D4C-BC39-6C3935D8163A}" name="Интерес" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A897308E-A602-47B1-B48B-4FD470549A10}" name="Интерес (пояснение)" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{C64844D7-2D5C-4311-9B26-83BA3A81B513}" name="Выбранная стратегия" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.IFS(AND(D2="Низкое",F2="Низкий"),"Наблюдать",AND(D2="Низкое",F2="Высокий"), "Информировать",AND(D2="Высокое",F2="Низкий"),"Поддерживать удовлетворённость",AND(D2="Высокое",F2="Высокий"),"Плотно работать")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -504,7 +501,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +673,7 @@
       <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="2" t="str">
+      <c r="H6" s="1" t="str">
         <f>_xlfn.IFS(AND(D6="Низкое",F6="Низкий"),"Наблюдать",AND(D6="Низкое",F6="Высокий"), "Информировать",AND(D6="Высокое",F6="Низкий"),"Поддерживать удовлетворённость",AND(D6="Высокое",F6="Высокий"),"Плотно работать")</f>
         <v>Информировать</v>
       </c>

</xml_diff>